<commit_message>
rename search variable, Excel update
</commit_message>
<xml_diff>
--- a/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702B5368-BF67-4DAD-8DCF-8AB845F435E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF2B3B4-6A3C-4182-BFF1-C045F788A560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6345" yWindow="2625" windowWidth="28905" windowHeight="15255" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="115">
   <si>
     <t>Informaţiile vor fi preluate din fişiere text.</t>
   </si>
@@ -524,6 +524,18 @@
   </si>
   <si>
     <t>93, 94,..., 93, 104, 105</t>
+  </si>
+  <si>
+    <t>searchItem</t>
+  </si>
+  <si>
+    <t>Part.Id == 1</t>
+  </si>
+  <si>
+    <t>Part.Name ==  "ZIMBABUE"</t>
+  </si>
+  <si>
+    <t>Part.Name == "ZIMBABUE"</t>
   </si>
 </sst>
 </file>
@@ -734,7 +746,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -815,19 +827,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1085,19 +1084,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color indexed="64"/>
       </left>
@@ -1197,7 +1183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1206,297 +1192,279 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1917,116 +1885,116 @@
   <dimension ref="B1:P20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B11"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="15" max="15" width="19.6640625" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="11"/>
-      <c r="D1" s="38" t="s">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B1" s="8"/>
+      <c r="D1" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="40"/>
-    </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="42"/>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="33" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="34" t="s">
+      <c r="N5" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26" t="s">
+      <c r="N6" s="22"/>
+      <c r="O6" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="P6" s="26" t="s">
+      <c r="P6" s="22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="N7" s="26" t="s">
+      <c r="N7" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="O7" s="26" t="s">
+      <c r="O7" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="P7" s="26">
+      <c r="P7" s="22">
         <v>234</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="N8" s="26" t="s">
+      <c r="N8" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="O8" s="26" t="s">
+      <c r="O8" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="P8" s="26">
+      <c r="P8" s="22">
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>79</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="N9" s="26" t="s">
+      <c r="N9" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="O9" s="26" t="s">
+      <c r="O9" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="P9" s="26">
+      <c r="P9" s="22">
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="102" t="s">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="35" t="s">
         <v>77</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>78</v>
       </c>
@@ -2034,15 +2002,15 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
     </row>
   </sheetData>
@@ -2061,119 +2029,119 @@
   </sheetPr>
   <dimension ref="B1:T24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" customWidth="1"/>
-    <col min="19" max="19" width="14.88671875" customWidth="1"/>
-    <col min="20" max="20" width="46.77734375" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" customWidth="1"/>
+    <col min="20" max="20" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B1" s="11"/>
-      <c r="D1" s="38" t="s">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B1" s="8"/>
+      <c r="D1" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="40"/>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B3" s="102" t="s">
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" s="35" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B6" s="38" t="s">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="I6" s="38" t="s">
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="I6" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="Q6" s="38" t="s">
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="Q6" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="R6" s="39"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="39"/>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B8" s="31" t="s">
+      <c r="R6" s="41"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="I8" s="11" t="s">
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="I8" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="Q8" s="43" t="s">
+      <c r="Q8" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="43"/>
-      <c r="S8" s="43"/>
-      <c r="T8" s="33">
+      <c r="R8" s="53"/>
+      <c r="S8" s="53"/>
+      <c r="T8" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B9" s="34" t="s">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="I9" s="36"/>
-      <c r="Q9" s="43" t="s">
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="I9" s="32"/>
+      <c r="Q9" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="R9" s="43"/>
-      <c r="S9" s="43"/>
-      <c r="T9" s="33" t="s">
+      <c r="R9" s="53"/>
+      <c r="S9" s="53"/>
+      <c r="T9" s="29" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B10" s="34" t="s">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
       <c r="I10" s="44"/>
       <c r="J10" s="45"/>
       <c r="K10" s="45"/>
@@ -2181,28 +2149,28 @@
       <c r="M10" s="45"/>
       <c r="N10" s="45"/>
       <c r="O10" s="46"/>
-      <c r="Q10" s="43" t="s">
+      <c r="Q10" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="R10" s="43" t="s">
+      <c r="R10" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="43"/>
-      <c r="T10" s="33">
+      <c r="S10" s="53"/>
+      <c r="T10" s="29">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B11" s="34" t="s">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
       <c r="I11" s="47"/>
       <c r="J11" s="48"/>
       <c r="K11" s="48"/>
@@ -2211,17 +2179,17 @@
       <c r="N11" s="48"/>
       <c r="O11" s="49"/>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="34" t="s">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
       <c r="I12" s="47"/>
       <c r="J12" s="48"/>
       <c r="K12" s="48"/>
@@ -2230,17 +2198,17 @@
       <c r="N12" s="48"/>
       <c r="O12" s="49"/>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B13" s="34" t="s">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
       <c r="I13" s="47"/>
       <c r="J13" s="48"/>
       <c r="K13" s="48"/>
@@ -2248,24 +2216,24 @@
       <c r="M13" s="48"/>
       <c r="N13" s="48"/>
       <c r="O13" s="49"/>
-      <c r="Q13" s="38" t="s">
+      <c r="Q13" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="R13" s="39"/>
-      <c r="S13" s="39"/>
-      <c r="T13" s="39"/>
-    </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B14" s="34" t="s">
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
       <c r="I14" s="47"/>
       <c r="J14" s="48"/>
       <c r="K14" s="48"/>
@@ -2274,7 +2242,7 @@
       <c r="N14" s="48"/>
       <c r="O14" s="49"/>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I15" s="47"/>
       <c r="J15" s="48"/>
       <c r="K15" s="48"/>
@@ -2282,16 +2250,16 @@
       <c r="M15" s="48"/>
       <c r="N15" s="48"/>
       <c r="O15" s="49"/>
-      <c r="Q15" s="31" t="s">
+      <c r="Q15" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="R15" s="53" t="s">
+      <c r="R15" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="S15" s="53"/>
-      <c r="T15" s="53"/>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="S15" s="54"/>
+      <c r="T15" s="54"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I16" s="47"/>
       <c r="J16" s="48"/>
       <c r="K16" s="48"/>
@@ -2299,16 +2267,16 @@
       <c r="M16" s="48"/>
       <c r="N16" s="48"/>
       <c r="O16" s="49"/>
-      <c r="Q16" s="34" t="s">
+      <c r="Q16" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="R16" s="41" t="s">
+      <c r="R16" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="S16" s="41"/>
-      <c r="T16" s="41"/>
-    </row>
-    <row r="17" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="S16" s="59"/>
+      <c r="T16" s="59"/>
+    </row>
+    <row r="17" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I17" s="47"/>
       <c r="J17" s="48"/>
       <c r="K17" s="48"/>
@@ -2316,16 +2284,16 @@
       <c r="M17" s="48"/>
       <c r="N17" s="48"/>
       <c r="O17" s="49"/>
-      <c r="Q17" s="34" t="s">
+      <c r="Q17" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="R17" s="103" t="s">
+      <c r="R17" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="S17" s="103"/>
-      <c r="T17" s="103"/>
-    </row>
-    <row r="18" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="S17" s="55"/>
+      <c r="T17" s="55"/>
+    </row>
+    <row r="18" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I18" s="47"/>
       <c r="J18" s="48"/>
       <c r="K18" s="48"/>
@@ -2333,16 +2301,16 @@
       <c r="M18" s="48"/>
       <c r="N18" s="48"/>
       <c r="O18" s="49"/>
-      <c r="Q18" s="34" t="s">
+      <c r="Q18" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="R18" s="41" t="s">
+      <c r="R18" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="S18" s="41"/>
-      <c r="T18" s="41"/>
-    </row>
-    <row r="19" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="S18" s="59"/>
+      <c r="T18" s="59"/>
+    </row>
+    <row r="19" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I19" s="47"/>
       <c r="J19" s="48"/>
       <c r="K19" s="48"/>
@@ -2350,16 +2318,16 @@
       <c r="M19" s="48"/>
       <c r="N19" s="48"/>
       <c r="O19" s="49"/>
-      <c r="Q19" s="34" t="s">
+      <c r="Q19" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="R19" s="104" t="s">
+      <c r="R19" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="S19" s="105"/>
-      <c r="T19" s="106"/>
-    </row>
-    <row r="20" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="S19" s="57"/>
+      <c r="T19" s="58"/>
+    </row>
+    <row r="20" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I20" s="47"/>
       <c r="J20" s="48"/>
       <c r="K20" s="48"/>
@@ -2368,7 +2336,7 @@
       <c r="N20" s="48"/>
       <c r="O20" s="49"/>
     </row>
-    <row r="21" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I21" s="47"/>
       <c r="J21" s="48"/>
       <c r="K21" s="48"/>
@@ -2377,7 +2345,7 @@
       <c r="N21" s="48"/>
       <c r="O21" s="49"/>
     </row>
-    <row r="22" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I22" s="47"/>
       <c r="J22" s="48"/>
       <c r="K22" s="48"/>
@@ -2386,7 +2354,7 @@
       <c r="N22" s="48"/>
       <c r="O22" s="49"/>
     </row>
-    <row r="23" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I23" s="47"/>
       <c r="J23" s="48"/>
       <c r="K23" s="48"/>
@@ -2395,7 +2363,7 @@
       <c r="N23" s="48"/>
       <c r="O23" s="49"/>
     </row>
-    <row r="24" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I24" s="50"/>
       <c r="J24" s="51"/>
       <c r="K24" s="51"/>
@@ -2406,6 +2374,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="R18:T18"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="I10:O24"/>
@@ -2422,11 +2395,6 @@
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="Q9:S9"/>
     <mergeCell ref="R16:T16"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="R18:T18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2441,54 +2409,54 @@
   </sheetPr>
   <dimension ref="B1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="4" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" customWidth="1"/>
-    <col min="8" max="8" width="18.77734375" customWidth="1"/>
-    <col min="9" max="9" width="23.77734375" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="21.21875" customWidth="1"/>
-    <col min="12" max="12" width="11.21875" customWidth="1"/>
-    <col min="13" max="13" width="26.77734375" customWidth="1"/>
-    <col min="14" max="14" width="8.77734375" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" customWidth="1"/>
-    <col min="19" max="19" width="9.109375" customWidth="1"/>
-    <col min="20" max="20" width="2.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="2.21875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="13" max="13" width="26.7109375" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" customWidth="1"/>
+    <col min="20" max="20" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B1" s="11"/>
-      <c r="D1" s="38" t="s">
+    <row r="1" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B1" s="8"/>
+      <c r="D1" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="40"/>
-    </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B4" s="102" t="s">
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="42"/>
+    </row>
+    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B4" s="35" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="2:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="60" t="s">
         <v>27</v>
       </c>
@@ -2523,400 +2491,411 @@
       <c r="Y6" s="60"/>
       <c r="Z6" s="60"/>
     </row>
-    <row r="7" spans="2:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="60"/>
       <c r="C7" s="60"/>
       <c r="D7" s="62"/>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="107" t="s">
+      <c r="F7" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="108"/>
-      <c r="H7" s="108"/>
-      <c r="I7" s="108"/>
-      <c r="J7" s="108"/>
-      <c r="K7" s="108"/>
-      <c r="L7" s="108"/>
-      <c r="M7" s="108"/>
-      <c r="N7" s="58" t="s">
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="O7" s="58"/>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="58"/>
-      <c r="R7" s="58"/>
-      <c r="S7" s="58"/>
-      <c r="T7" s="59" t="s">
+      <c r="O7" s="64"/>
+      <c r="P7" s="64"/>
+      <c r="Q7" s="64"/>
+      <c r="R7" s="64"/>
+      <c r="S7" s="64"/>
+      <c r="T7" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="U7" s="59"/>
-      <c r="V7" s="59"/>
-      <c r="W7" s="59"/>
-      <c r="X7" s="59"/>
-      <c r="Y7" s="59"/>
-      <c r="Z7" s="59"/>
-    </row>
-    <row r="8" spans="2:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U7" s="63"/>
+      <c r="V7" s="63"/>
+      <c r="W7" s="63"/>
+      <c r="X7" s="63"/>
+      <c r="Y7" s="63"/>
+      <c r="Z7" s="63"/>
+    </row>
+    <row r="8" spans="2:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="60"/>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="D8" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="57"/>
-      <c r="F8" s="56" t="s">
+      <c r="E8" s="68"/>
+      <c r="F8" s="67" t="s">
         <v>98</v>
       </c>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56" t="s">
+      <c r="G8" s="67"/>
+      <c r="H8" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="I8" s="56"/>
-      <c r="J8" s="56" t="s">
+      <c r="I8" s="67"/>
+      <c r="J8" s="67" t="s">
         <v>96</v>
       </c>
-      <c r="K8" s="56"/>
-      <c r="L8" s="56" t="s">
+      <c r="K8" s="67"/>
+      <c r="L8" s="67" t="s">
         <v>97</v>
       </c>
-      <c r="M8" s="56"/>
-      <c r="N8" s="58" t="s">
+      <c r="M8" s="67"/>
+      <c r="N8" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="O8" s="58" t="s">
+      <c r="O8" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="P8" s="58" t="s">
+      <c r="P8" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="Q8" s="58" t="s">
+      <c r="Q8" s="64" t="s">
         <v>99</v>
       </c>
-      <c r="R8" s="58" t="s">
+      <c r="R8" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="S8" s="58" t="s">
+      <c r="S8" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="T8" s="59">
+      <c r="T8" s="63">
         <v>0</v>
       </c>
-      <c r="U8" s="59">
+      <c r="U8" s="63">
         <v>1</v>
       </c>
-      <c r="V8" s="59">
+      <c r="V8" s="63">
         <v>2</v>
       </c>
-      <c r="W8" s="59" t="s">
+      <c r="W8" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="X8" s="59" t="s">
+      <c r="X8" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="Y8" s="59" t="s">
+      <c r="Y8" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="Z8" s="59" t="s">
+      <c r="Z8" s="63" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="2:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="60"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="12" t="s">
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="L9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M9" s="12" t="s">
+      <c r="M9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="N9" s="58"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="58"/>
-      <c r="Q9" s="58"/>
-      <c r="R9" s="58"/>
-      <c r="S9" s="58"/>
-      <c r="T9" s="59"/>
-      <c r="U9" s="59"/>
-      <c r="V9" s="59"/>
-      <c r="W9" s="59"/>
-      <c r="X9" s="59"/>
-      <c r="Y9" s="59"/>
-      <c r="Z9" s="59"/>
-    </row>
-    <row r="10" spans="2:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="13" t="s">
+      <c r="N9" s="64"/>
+      <c r="O9" s="64"/>
+      <c r="P9" s="64"/>
+      <c r="Q9" s="64"/>
+      <c r="R9" s="64"/>
+      <c r="S9" s="64"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="63"/>
+      <c r="V9" s="63"/>
+      <c r="W9" s="63"/>
+      <c r="X9" s="63"/>
+      <c r="Y9" s="63"/>
+      <c r="Z9" s="63"/>
+    </row>
+    <row r="10" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16" t="s">
+      <c r="F10" s="13"/>
+      <c r="G10" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17" t="s">
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="18" t="s">
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="18"/>
-      <c r="Z10" s="18"/>
-    </row>
-    <row r="11" spans="2:26" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B11" s="13" t="s">
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
+    </row>
+    <row r="11" spans="2:26" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16" t="s">
+      <c r="G11" s="13"/>
+      <c r="H11" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16" t="s">
+      <c r="J11" s="13"/>
+      <c r="K11" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="L11" s="16" t="s">
+      <c r="L11" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="M11" s="16"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17" t="s">
+      <c r="M11" s="13"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18" t="s">
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="18"/>
-    </row>
-    <row r="12" spans="2:26" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B12" s="13" t="s">
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+    </row>
+    <row r="12" spans="2:26" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C12" s="109" t="s">
+      <c r="C12" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="D12" s="110" t="s">
+      <c r="D12" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16" t="s">
+      <c r="G12" s="13"/>
+      <c r="H12" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="I12" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="J12" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="17" t="s">
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18" t="s">
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="18"/>
-      <c r="Z12" s="18"/>
-    </row>
-    <row r="13" spans="2:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="13" t="s">
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+    </row>
+    <row r="13" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16" t="s">
+      <c r="J13" s="13"/>
+      <c r="K13" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16" t="s">
+      <c r="L13" s="13"/>
+      <c r="M13" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17" t="s">
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18" t="s">
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="Z13" s="18"/>
-    </row>
-    <row r="14" spans="2:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="13" t="s">
+      <c r="Z13" s="15"/>
+    </row>
+    <row r="14" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="18"/>
-    </row>
-    <row r="15" spans="2:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B15" s="13" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+    </row>
+    <row r="15" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
-      <c r="W15" s="18"/>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="18"/>
-      <c r="Z15" s="18"/>
-    </row>
-    <row r="16" spans="2:26" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="19"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="15"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="15"/>
+    </row>
+    <row r="16" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="N7:S7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="C6:C7"/>
@@ -2933,17 +2912,6 @@
     <mergeCell ref="R8:R9"/>
     <mergeCell ref="T7:Z7"/>
     <mergeCell ref="Z8:Z9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="N7:S7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2955,427 +2923,315 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:N16"/>
+  <dimension ref="B1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" customWidth="1"/>
+    <col min="7" max="7" width="31.85546875" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" customWidth="1"/>
-    <col min="13" max="13" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B1" s="11"/>
-      <c r="D1" s="38" t="s">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="8"/>
+      <c r="D1" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="40"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="88" t="s">
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="42"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="89" t="s">
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="103"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="D4" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="82" t="s">
+      <c r="E4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="93"/>
-      <c r="I4" s="93"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="82" t="s">
+      <c r="F4" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="83"/>
-    </row>
-    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="90"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="96"/>
+      <c r="G4" s="72"/>
+    </row>
+    <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="70"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="77"/>
       <c r="E5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="17">
+        <v>9</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="17">
+        <v>10</v>
+      </c>
+      <c r="C7" s="73"/>
+      <c r="D7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="17">
+        <v>11</v>
+      </c>
+      <c r="C8" s="73"/>
+      <c r="D8" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="17">
+        <v>12</v>
+      </c>
+      <c r="C9" s="73"/>
+      <c r="D9" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="19"/>
+    </row>
+    <row r="12" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="80" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="99" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="100"/>
+      <c r="H12" s="80" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="81"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="N12" s="88"/>
+    </row>
+    <row r="13" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="86" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="78" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="90" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="94" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="95" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="97" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="M13" s="85" t="s">
+        <v>72</v>
+      </c>
+      <c r="N13" s="74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="89"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="93"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="96"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="79"/>
+      <c r="K14" s="98"/>
+      <c r="L14" s="84"/>
+      <c r="M14" s="86"/>
+      <c r="N14" s="92"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="22">
+        <v>4</v>
+      </c>
+      <c r="C15" s="20">
+        <v>4</v>
+      </c>
+      <c r="D15" s="20">
+        <v>0</v>
+      </c>
+      <c r="E15" s="104">
         <v>1</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="84" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="85"/>
-      <c r="K5" s="2" t="s">
+      <c r="F15" s="21"/>
+      <c r="G15" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="22">
+        <f>SUM(J15:K15)</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="20">
+        <v>0</v>
+      </c>
+      <c r="K15" s="23">
+        <v>0</v>
+      </c>
+      <c r="L15" s="24"/>
+      <c r="M15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="N15" s="25">
+        <f>C15</f>
         <v>4</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="20">
-        <v>9</v>
-      </c>
-      <c r="C6" s="91" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="80" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="81"/>
-      <c r="K6" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" s="20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="20">
-        <v>10</v>
-      </c>
-      <c r="C7" s="91"/>
-      <c r="D7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="20">
-        <v>5</v>
-      </c>
-      <c r="F7" s="20">
-        <v>6</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" s="83"/>
-      <c r="K7" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7" s="20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="20">
-        <v>11</v>
-      </c>
-      <c r="C8" s="91"/>
-      <c r="D8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" s="83"/>
-      <c r="K8" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="L8" s="20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="20">
-        <v>12</v>
-      </c>
-      <c r="C9" s="91"/>
-      <c r="D9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="83"/>
-      <c r="K9" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9" s="20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="2">
-        <v>13</v>
-      </c>
-      <c r="C10" s="92"/>
-      <c r="D10" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" s="84" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" s="85"/>
-      <c r="K10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="22"/>
-    </row>
-    <row r="13" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="97" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="99" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="100"/>
-      <c r="H13" s="97" t="s">
-        <v>65</v>
-      </c>
-      <c r="I13" s="98"/>
-      <c r="J13" s="98"/>
-      <c r="K13" s="98"/>
-      <c r="L13" s="101"/>
-      <c r="M13" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="N13" s="68"/>
-    </row>
-    <row r="14" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="66" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="70" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="70" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="72" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="74" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" s="76" t="s">
-        <v>69</v>
-      </c>
-      <c r="H14" s="78" t="s">
-        <v>70</v>
-      </c>
-      <c r="I14" s="70" t="s">
-        <v>39</v>
-      </c>
-      <c r="J14" s="70" t="s">
-        <v>40</v>
-      </c>
-      <c r="K14" s="86" t="s">
-        <v>42</v>
-      </c>
-      <c r="L14" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="M14" s="65" t="s">
-        <v>72</v>
-      </c>
-      <c r="N14" s="77" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="69"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="71"/>
-      <c r="K15" s="87"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="66"/>
-      <c r="N15" s="74"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="26">
-        <f>SUM(C16:D16)</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="23">
-        <v>0</v>
-      </c>
-      <c r="D16" s="23">
-        <v>0</v>
-      </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="I16" s="26">
-        <f>SUM(J16:K16)</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="23">
-        <v>0</v>
-      </c>
-      <c r="K16" s="27">
-        <v>0</v>
-      </c>
-      <c r="L16" s="28"/>
-      <c r="M16" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="N16" s="29">
-        <f>C16</f>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="24">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="M12:N12"/>
     <mergeCell ref="D1:G1"/>
-    <mergeCell ref="B3:L3"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="C6:C9"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3383,12 +3239,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3536,15 +3389,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFB6F214-3FD3-47D7-BFB6-77D735E8F784}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC4FB184-C14D-4C2C-BD91-7F8240B2478B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3568,10 +3425,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC4FB184-C14D-4C2C-BD91-7F8240B2478B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFB6F214-3FD3-47D7-BFB6-77D735E8F784}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>